<commit_message>
improved auto_sequence function, included in a object
The previous problem was that some copies of used lists wasn't independant. This was making the results wrongs. This issue has been solved with the new auto_sequence function
</commit_message>
<xml_diff>
--- a/Interface.xlsx
+++ b/Interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\Projet Siemens\Python entrainement\Turbine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13685EE0-66DD-4C38-B4F8-5EE7DA0D60F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C3B32B-2AEF-4E2A-8A01-B14A2794DD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10644" yWindow="1464" windowWidth="12396" windowHeight="10848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -789,7 +789,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
ajout comparaison performances dans affichage
</commit_message>
<xml_diff>
--- a/Interface.xlsx
+++ b/Interface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\Projet Siemens\Python entrainement\Turbine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8E8A63-F7C7-42F8-A53F-A91B427F8EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A6DE32-C29F-4E2F-B7BC-E687A92E1AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10644" yWindow="1464" windowWidth="12396" windowHeight="10848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -935,7 +935,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,25 +1597,25 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A2:B47">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>$E$9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>$E$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>$E$7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>$E$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>$E$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
       <formula>$E$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
correction affichage comparaison SFC
</commit_message>
<xml_diff>
--- a/Interface.xlsx
+++ b/Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\Projet Siemens\Python entrainement\Turbine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A6DE32-C29F-4E2F-B7BC-E687A92E1AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8D673F-E42A-4C03-AB9E-B4D783F449D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -235,19 +235,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -361,9 +348,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -372,12 +363,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -388,10 +377,21 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -412,70 +412,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -484,13 +466,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -535,70 +517,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -935,7 +935,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,637 +951,637 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="51" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="53"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="28">
+      <c r="A2" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B2" s="43">
+      <c r="B2" s="37">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="3" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="58" t="s">
+      <c r="F2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="59"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="28">
+      <c r="A3" s="22">
         <v>2</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="37">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6">
+      <c r="C3" s="8"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="48">
         <v>1</v>
       </c>
-      <c r="F3" s="60" t="s">
+      <c r="F3" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="61"/>
+      <c r="G3" s="58"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="28">
+      <c r="A4" s="22">
         <v>5.2</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="37">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="7">
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="49">
         <v>2</v>
       </c>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="63"/>
+      <c r="G4" s="60"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="28">
+      <c r="A5" s="22">
         <v>3</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="37">
         <v>3</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="50">
         <v>3</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="65"/>
+      <c r="G5" s="62"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="43">
+      <c r="A6" s="22"/>
+      <c r="B6" s="37">
         <v>4.2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="15">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="45">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F6" s="54" t="s">
+      <c r="F6" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="55"/>
+      <c r="G6" s="52"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="15">
+      <c r="A7" s="22"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="45">
         <v>4.2</v>
       </c>
-      <c r="F7" s="54" t="s">
+      <c r="F7" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="52"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="17">
+      <c r="A8" s="22"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="46">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="57"/>
+      <c r="G8" s="54"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="17">
+      <c r="A9" s="22"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="46">
         <v>5.2</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="F9" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="57"/>
+      <c r="G9" s="54"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="8"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="43"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="30" t="s">
+      <c r="A12" s="22"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="12">
         <v>1</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="12">
         <v>288</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="20"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="20"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="32" t="s">
+      <c r="A17" s="22"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="32" t="str">
+      <c r="F17" s="26" t="str">
         <f>F12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G17" s="45" t="str">
+      <c r="G17" s="39" t="str">
         <f>G12</f>
         <v>Séquence 2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="9">
+      <c r="F18" s="12"/>
+      <c r="G18" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="43"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="10">
+      <c r="F19" s="34"/>
+      <c r="G19" s="6">
         <v>0.99</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="10">
+      <c r="F20" s="34"/>
+      <c r="G20" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="20"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="14"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="37"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="33" t="s">
+      <c r="A23" s="22"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="33" t="str">
+      <c r="F23" s="27" t="str">
         <f>F12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G23" s="46" t="str">
+      <c r="G23" s="40" t="str">
         <f>G12</f>
         <v>Séquence 2</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="12">
         <v>1350</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="5">
         <v>1100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="34">
         <v>0.99</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25" s="6">
         <v>0.98</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
+      <c r="A26" s="22"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="40">
+      <c r="F26" s="34">
         <v>0.06</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26" s="6">
         <v>0.02</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="8"/>
+      <c r="A27" s="22"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="8"/>
+      <c r="A28" s="22"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="34" t="s">
+      <c r="A29" s="22"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="34" t="str">
+      <c r="F29" s="28" t="str">
         <f>F12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G29" s="47" t="str">
+      <c r="G29" s="41" t="str">
         <f>G12</f>
         <v>Séquence 2</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="34">
         <v>0.99</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
+      <c r="A31" s="22"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="E31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="34">
         <v>0.89</v>
       </c>
-      <c r="G31" s="10">
+      <c r="G31" s="6">
         <v>0.87</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="35">
         <v>0.03</v>
       </c>
-      <c r="G32" s="16">
+      <c r="G32" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="23"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="43"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="8"/>
+      <c r="A34" s="22"/>
+      <c r="B34" s="37"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="37" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="35" t="str">
+      <c r="F35" s="29" t="str">
         <f>F12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G35" s="48" t="str">
+      <c r="G35" s="42" t="str">
         <f>G12</f>
         <v>Séquence 2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="43"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4" t="s">
+      <c r="A36" s="22"/>
+      <c r="B36" s="37"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="10">
+      <c r="F36" s="34"/>
+      <c r="G36" s="6">
         <v>0.8</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
-      <c r="B37" s="43"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4" t="s">
+      <c r="A37" s="22"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="10">
+      <c r="F37" s="34"/>
+      <c r="G37" s="6">
         <v>0.03</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="43"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4" t="s">
+      <c r="A38" s="22"/>
+      <c r="B38" s="37"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="41"/>
-      <c r="G38" s="16">
+      <c r="F38" s="35"/>
+      <c r="G38" s="11">
         <v>0.04</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="43"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="8"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="43"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="8"/>
+      <c r="A40" s="22"/>
+      <c r="B40" s="37"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="4"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="38" t="s">
+      <c r="A41" s="22"/>
+      <c r="B41" s="37"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="31" t="str">
+      <c r="F41" s="25" t="str">
         <f>F12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G41" s="49" t="str">
+      <c r="G41" s="43" t="str">
         <f>G12</f>
         <v>Séquence 2</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="43"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4" t="s">
+      <c r="A42" s="22"/>
+      <c r="B42" s="37"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="18">
+      <c r="F42" s="12">
         <v>12</v>
       </c>
-      <c r="G42" s="9"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4" t="s">
+      <c r="A43" s="22"/>
+      <c r="B43" s="37"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="40">
+      <c r="F43" s="34">
         <v>0.99</v>
       </c>
-      <c r="G43" s="10"/>
-      <c r="H43" s="4"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="43"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4" t="s">
+      <c r="A44" s="22"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="40">
+      <c r="F44" s="34">
         <v>0.86</v>
       </c>
-      <c r="G44" s="10"/>
-      <c r="H44" s="4"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="43"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4" t="s">
+      <c r="A45" s="22"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="40">
+      <c r="F45" s="34">
         <v>0.89</v>
       </c>
-      <c r="G45" s="10"/>
-      <c r="H45" s="4"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="4"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="29"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="21"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="15"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
     </row>
     <row r="49" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
     <row r="50" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
     </row>
     <row r="51" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1634,111 +1634,111 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="25"/>
-    <col min="3" max="3" width="21.33203125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="25"/>
+    <col min="1" max="2" width="11.5546875" style="19"/>
+    <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <f>user!F13</f>
         <v>1</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <f>user!F18</f>
         <v>0</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="10">
         <f>user!F24</f>
         <v>1350</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="10">
         <f>user!F30</f>
         <v>0.99</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="10">
         <f>user!F36</f>
         <v>0</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="19">
         <f>user!F42</f>
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <f>user!F14</f>
         <v>288</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <f>user!F19</f>
         <v>0</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <f>user!F25</f>
         <v>0.99</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <f>user!F31</f>
         <v>0.89</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <f>user!F37</f>
         <v>0</v>
       </c>
-      <c r="F3" s="25">
+      <c r="F3" s="19">
         <f>user!F43</f>
         <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10">
         <f>user!F20</f>
         <v>0</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <f>user!F26</f>
         <v>0.06</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <f>user!F32</f>
         <v>0.03</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <f>user!F38</f>
         <v>0</v>
       </c>
-      <c r="F4" s="25">
+      <c r="F4" s="19">
         <f>user!F44</f>
         <v>0.86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" s="25">
+      <c r="F5" s="19">
         <f>user!F45</f>
         <v>0.89</v>
       </c>
@@ -1758,111 +1758,111 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="25"/>
-    <col min="3" max="3" width="21.33203125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="25" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="25"/>
+    <col min="1" max="2" width="11.5546875" style="19"/>
+    <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="19" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="19" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="14">
+      <c r="A2" s="10">
         <f>user!G13</f>
         <v>1</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="10">
         <f>user!G18</f>
         <v>4</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="10">
         <f>user!G24</f>
         <v>1100</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="10">
         <f>user!G30</f>
         <v>1</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="10">
         <f>user!G36</f>
         <v>0.8</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="19">
         <f>user!G42</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="14">
+      <c r="A3" s="10">
         <f>user!G14</f>
         <v>288</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="10">
         <f>user!G19</f>
         <v>0.99</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="10">
         <f>user!G25</f>
         <v>0.98</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="10">
         <f>user!G31</f>
         <v>0.87</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="10">
         <f>user!G37</f>
         <v>0.03</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="36">
         <f>user!G43</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10">
         <f>user!G20</f>
         <v>0.85</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="10">
         <f>user!G26</f>
         <v>0.02</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="10">
         <f>user!G32</f>
         <v>0</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="10">
         <f>user!G38</f>
         <v>0.04</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="36">
         <f>user!G44</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" s="42">
+      <c r="F5" s="36">
         <f>user!G45</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
possiblité de nommer sur xl interface
</commit_message>
<xml_diff>
--- a/Interface.xlsx
+++ b/Interface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Desktop\Projet Siemens\Python entrainement\Turbine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8D673F-E42A-4C03-AB9E-B4D783F449D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC08C6-6333-4301-B19C-4F656113D55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Compresseur</t>
   </si>
@@ -117,13 +117,25 @@
   </si>
   <si>
     <t>Exhaust pressure loss (bar</t>
+  </si>
+  <si>
+    <t>Nom cycles</t>
+  </si>
+  <si>
+    <t>Saisir codes pour séquence cycle</t>
+  </si>
+  <si>
+    <t>Cycle avec Échangeur de chaleur</t>
+  </si>
+  <si>
+    <t>Cycle Gas generator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +168,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -211,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -292,36 +311,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -397,6 +386,43 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -442,13 +468,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -469,12 +492,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -514,10 +531,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -535,9 +549,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -556,6 +567,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -590,15 +625,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -932,691 +958,744 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="8" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="25.21875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="21.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="8" style="1" customWidth="1"/>
+    <col min="6" max="6" width="43.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="9"/>
+    <row r="1" spans="1:8" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>32</v>
+      </c>
       <c r="D1" s="9"/>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="64"/>
-      <c r="G1" s="65"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="22">
+      <c r="G1" s="52"/>
+      <c r="H1" s="53"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="12">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B2" s="37">
+      <c r="C2" s="12">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="47" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="55" t="s">
+      <c r="G2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="56"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="22">
+      <c r="H2" s="59"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="49"/>
+      <c r="B3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="37">
+      <c r="C3" s="12">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="48">
+      <c r="D3" s="8"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="43">
         <v>1</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="G3" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="58"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="22">
+      <c r="H3" s="61"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
+      <c r="B4" s="12">
         <v>5.2</v>
       </c>
-      <c r="B4" s="37">
+      <c r="C4" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="49">
+      <c r="E4" s="3"/>
+      <c r="F4" s="44">
         <v>2</v>
       </c>
-      <c r="F4" s="59" t="s">
+      <c r="G4" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="60"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="22">
+      <c r="H4" s="63"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
+      <c r="B5" s="12">
         <v>3</v>
       </c>
-      <c r="B5" s="37">
+      <c r="C5" s="12">
         <v>3</v>
       </c>
-      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="50">
+      <c r="E5" s="3"/>
+      <c r="F5" s="45">
         <v>3</v>
       </c>
-      <c r="F5" s="61" t="s">
+      <c r="G5" s="64" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="62"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
-      <c r="B6" s="37">
+      <c r="H5" s="65"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12">
         <v>4.2</v>
       </c>
-      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="45">
+      <c r="E6" s="3"/>
+      <c r="F6" s="40">
         <v>4.0999999999999996</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="G6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="52"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
-      <c r="B7" s="37"/>
-      <c r="C7" s="3"/>
+      <c r="H6" s="55"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="45">
+      <c r="E7" s="3"/>
+      <c r="F7" s="40">
         <v>4.2</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="G7" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="52"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="3"/>
+      <c r="H7" s="55"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="46">
+      <c r="E8" s="3"/>
+      <c r="F8" s="41">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F8" s="53" t="s">
+      <c r="G8" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="54"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="3"/>
+      <c r="H8" s="57"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="46">
+      <c r="E9" s="3"/>
+      <c r="F9" s="41">
         <v>5.2</v>
       </c>
-      <c r="F9" s="53" t="s">
+      <c r="G9" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="54"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="37"/>
-      <c r="C10" s="3"/>
+      <c r="H9" s="57"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="49"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="49"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="3"/>
+      <c r="F12" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="H12" s="20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="3"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="12">
+      <c r="G13" s="12">
         <v>1</v>
       </c>
-      <c r="G13" s="5">
+      <c r="H13" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="12">
+      <c r="G14" s="12">
         <v>288</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="3"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="26" t="s">
+      <c r="E17" s="3"/>
+      <c r="F17" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="26" t="str">
-        <f>F12</f>
+      <c r="G17" s="23" t="str">
+        <f>G12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G17" s="39" t="str">
-        <f>G12</f>
+      <c r="H17" s="35" t="str">
+        <f>H12</f>
         <v>Séquence 2</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="3"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="5">
+      <c r="G18" s="12"/>
+      <c r="H18" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="3"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3"/>
+      <c r="F19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F19" s="34"/>
-      <c r="G19" s="6">
+      <c r="G19" s="31"/>
+      <c r="H19" s="6">
         <v>0.99</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="3"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="6">
+      <c r="G20" s="31"/>
+      <c r="H20" s="6">
         <v>0.85</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="3"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="14"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="37"/>
-      <c r="C22" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="49"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
-      <c r="B23" s="37"/>
-      <c r="C23" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="27" t="s">
+      <c r="E23" s="3"/>
+      <c r="F23" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F23" s="27" t="str">
-        <f>F12</f>
+      <c r="G23" s="24" t="str">
+        <f>G12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G23" s="40" t="str">
-        <f>G12</f>
+      <c r="H23" s="36" t="str">
+        <f>H12</f>
         <v>Séquence 2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="3"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="49"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="12">
+      <c r="G24" s="12">
         <v>1350</v>
       </c>
-      <c r="G24" s="5">
+      <c r="H24" s="5">
         <v>1100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="3"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="49"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3"/>
+      <c r="F25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="34">
+      <c r="G25" s="31">
         <v>0.99</v>
       </c>
-      <c r="G25" s="6">
+      <c r="H25" s="6">
         <v>0.98</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="3"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F26" s="34">
+      <c r="G26" s="31">
         <v>0.06</v>
       </c>
-      <c r="G26" s="6">
+      <c r="H26" s="6">
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
-      <c r="B27" s="37"/>
-      <c r="C27" s="3"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="4"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="49"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
-      <c r="B29" s="37"/>
-      <c r="C29" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="49"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="28" t="str">
-        <f>F12</f>
+      <c r="G29" s="25" t="str">
+        <f>G12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G29" s="41" t="str">
-        <f>G12</f>
+      <c r="H29" s="37" t="str">
+        <f>H12</f>
         <v>Séquence 2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
-      <c r="B30" s="37"/>
-      <c r="C30" s="3"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="49"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="34">
+      <c r="G30" s="31">
         <v>0.99</v>
       </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="3"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="49"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="2" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="34">
+      <c r="G31" s="31">
         <v>0.89</v>
       </c>
-      <c r="G31" s="6">
+      <c r="H31" s="6">
         <v>0.87</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
-      <c r="B32" s="37"/>
-      <c r="C32" s="3"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="35">
+      <c r="G32" s="32">
         <v>0.03</v>
       </c>
-      <c r="G32" s="11">
+      <c r="H32" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="3"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="49"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="49"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="49"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="31" t="s">
+      <c r="E35" s="3"/>
+      <c r="F35" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="29" t="str">
-        <f>F12</f>
+      <c r="G35" s="26" t="str">
+        <f>G12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G35" s="42" t="str">
-        <f>G12</f>
+      <c r="H35" s="38" t="str">
+        <f>H12</f>
         <v>Séquence 2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="3"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="49"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="3"/>
+      <c r="F36" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="34"/>
-      <c r="G36" s="6">
+      <c r="G36" s="31"/>
+      <c r="H36" s="6">
         <v>0.8</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
-      <c r="B37" s="37"/>
-      <c r="C37" s="3"/>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="49"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="34"/>
-      <c r="G37" s="6">
+      <c r="G37" s="31"/>
+      <c r="H37" s="6">
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
-      <c r="B38" s="37"/>
-      <c r="C38" s="3"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="49"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F38" s="35"/>
-      <c r="G38" s="11">
+      <c r="G38" s="32"/>
+      <c r="H38" s="11">
         <v>0.04</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
-      <c r="B39" s="37"/>
-      <c r="C39" s="3"/>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="49"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="49"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="3"/>
+      <c r="F41" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="25" t="str">
-        <f>F12</f>
+      <c r="G41" s="22" t="str">
+        <f>G12</f>
         <v>Séquence 1</v>
       </c>
-      <c r="G41" s="43" t="str">
-        <f>G12</f>
+      <c r="H41" s="39" t="str">
+        <f>H12</f>
         <v>Séquence 2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="3"/>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="49"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="12">
+      <c r="G42" s="12">
         <v>12</v>
       </c>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="3"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="49"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="3"/>
+      <c r="F43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F43" s="34">
+      <c r="G43" s="31">
         <v>0.99</v>
       </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="3"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="49"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="34">
+      <c r="G44" s="31">
         <v>0.86</v>
       </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="3"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="3"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="49"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="34">
+      <c r="G45" s="31">
         <v>0.89</v>
       </c>
-      <c r="G45" s="6"/>
-      <c r="H45" s="3"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
-      <c r="B46" s="37"/>
-      <c r="C46" s="3"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="49"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="33"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="3"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="23"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="7"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="50"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
-      <c r="G47" s="15"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E48" s="3"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F48" s="3"/>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F49" s="3"/>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E50" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E51" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A47"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A2:B47">
+  <conditionalFormatting sqref="B2:C47">
     <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>$E$9</formula>
+      <formula>$F$9</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>$E$8</formula>
+      <formula>$F$8</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
-      <formula>$E$7</formula>
+      <formula>$F$7</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
-      <formula>$E$6</formula>
+      <formula>$F$6</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="12" operator="equal">
-      <formula>$E$5</formula>
+      <formula>$F$5</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
-      <formula>$E$4</formula>
+      <formula>$F$4</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
-      <formula>$E$3</formula>
+      <formula>$F$3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1634,112 +1713,112 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="19"/>
-    <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="19"/>
+    <col min="1" max="2" width="11.5546875" style="18"/>
+    <col min="3" max="3" width="21.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
-        <f>user!F13</f>
+        <f>user!G13</f>
         <v>1</v>
       </c>
       <c r="B2" s="10">
-        <f>user!F18</f>
+        <f>user!G18</f>
         <v>0</v>
       </c>
       <c r="C2" s="10">
-        <f>user!F24</f>
+        <f>user!G24</f>
         <v>1350</v>
       </c>
       <c r="D2" s="10">
-        <f>user!F30</f>
+        <f>user!G30</f>
         <v>0.99</v>
       </c>
       <c r="E2" s="10">
-        <f>user!F36</f>
+        <f>user!G36</f>
         <v>0</v>
       </c>
-      <c r="F2" s="19">
-        <f>user!F42</f>
+      <c r="F2" s="18">
+        <f>user!G42</f>
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
-        <f>user!F14</f>
+        <f>user!G14</f>
         <v>288</v>
       </c>
       <c r="B3" s="10">
-        <f>user!F19</f>
+        <f>user!G19</f>
         <v>0</v>
       </c>
       <c r="C3" s="10">
-        <f>user!F25</f>
+        <f>user!G25</f>
         <v>0.99</v>
       </c>
       <c r="D3" s="10">
-        <f>user!F31</f>
+        <f>user!G31</f>
         <v>0.89</v>
       </c>
       <c r="E3" s="10">
-        <f>user!F37</f>
+        <f>user!G37</f>
         <v>0</v>
       </c>
-      <c r="F3" s="19">
-        <f>user!F43</f>
+      <c r="F3" s="18">
+        <f>user!G43</f>
         <v>0.99</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10">
-        <f>user!F20</f>
+        <f>user!G20</f>
         <v>0</v>
       </c>
       <c r="C4" s="10">
-        <f>user!F26</f>
+        <f>user!G26</f>
         <v>0.06</v>
       </c>
       <c r="D4" s="10">
-        <f>user!F32</f>
+        <f>user!G32</f>
         <v>0.03</v>
       </c>
       <c r="E4" s="10">
-        <f>user!F38</f>
+        <f>user!G38</f>
         <v>0</v>
       </c>
-      <c r="F4" s="19">
-        <f>user!F44</f>
+      <c r="F4" s="18">
+        <f>user!G44</f>
         <v>0.86</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" s="19">
-        <f>user!F45</f>
+      <c r="F5" s="18">
+        <f>user!G45</f>
         <v>0.89</v>
       </c>
     </row>
@@ -1758,112 +1837,112 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.5546875" style="19"/>
-    <col min="3" max="3" width="21.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="19" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" style="19" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="19"/>
+    <col min="1" max="2" width="11.5546875" style="18"/>
+    <col min="3" max="3" width="21.33203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="18" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="11.5546875" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="10">
-        <f>user!G13</f>
+        <f>user!H13</f>
         <v>1</v>
       </c>
       <c r="B2" s="10">
-        <f>user!G18</f>
+        <f>user!H18</f>
         <v>4</v>
       </c>
       <c r="C2" s="10">
-        <f>user!G24</f>
+        <f>user!H24</f>
         <v>1100</v>
       </c>
       <c r="D2" s="10">
-        <f>user!G30</f>
+        <f>user!H30</f>
         <v>1</v>
       </c>
       <c r="E2" s="10">
-        <f>user!G36</f>
+        <f>user!H36</f>
         <v>0.8</v>
       </c>
-      <c r="F2" s="19">
-        <f>user!G42</f>
+      <c r="F2" s="18">
+        <f>user!H42</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10">
-        <f>user!G14</f>
+        <f>user!H14</f>
         <v>288</v>
       </c>
       <c r="B3" s="10">
-        <f>user!G19</f>
+        <f>user!H19</f>
         <v>0.99</v>
       </c>
       <c r="C3" s="10">
-        <f>user!G25</f>
+        <f>user!H25</f>
         <v>0.98</v>
       </c>
       <c r="D3" s="10">
-        <f>user!G31</f>
+        <f>user!H31</f>
         <v>0.87</v>
       </c>
       <c r="E3" s="10">
-        <f>user!G37</f>
+        <f>user!H37</f>
         <v>0.03</v>
       </c>
-      <c r="F3" s="36">
-        <f>user!G43</f>
+      <c r="F3" s="33">
+        <f>user!H43</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
       <c r="B4" s="10">
-        <f>user!G20</f>
+        <f>user!H20</f>
         <v>0.85</v>
       </c>
       <c r="C4" s="10">
-        <f>user!G26</f>
+        <f>user!H26</f>
         <v>0.02</v>
       </c>
       <c r="D4" s="10">
-        <f>user!G32</f>
+        <f>user!H32</f>
         <v>0</v>
       </c>
       <c r="E4" s="10">
-        <f>user!G38</f>
+        <f>user!H38</f>
         <v>0.04</v>
       </c>
-      <c r="F4" s="36">
-        <f>user!G44</f>
+      <c r="F4" s="33">
+        <f>user!H44</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F5" s="36">
-        <f>user!G45</f>
+      <c r="F5" s="33">
+        <f>user!H45</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>